<commit_message>
EU27 Updated trans/BMRESP -- description changed in "about" tab
</commit_message>
<xml_diff>
--- a/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
+++ b/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\BMRESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\eps-eu\InputData\trans\BMRESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71892F56-767B-4735-B121-3FC3453AE43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="23955" windowHeight="12090"/>
+    <workbookView xWindow="1500" yWindow="90" windowWidth="16740" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -56,16 +57,16 @@
     <t>motorbikes</t>
   </si>
   <si>
-    <t>in the United States for any vehicle type.</t>
+    <t>Sales Percentage (dimensionless)</t>
   </si>
   <si>
-    <t>Sales Percentage (dimensionless)</t>
+    <t>in the European Union for any vehicle type.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -202,6 +203,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -237,6 +255,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,19 +447,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -432,19 +469,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -454,7 +491,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -462,14 +499,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <v>2016</v>
@@ -577,7 +614,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -687,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -797,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -907,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1017,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1243,7 +1280,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1251,14 +1288,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <v>2016</v>
@@ -1366,7 +1403,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1586,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1696,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1806,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1916,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>

</xml_diff>